<commit_message>
updating object positions and gestures for final tests
</commit_message>
<xml_diff>
--- a/data/gestures/Reachy_gestures/Key joint values.xlsx
+++ b/data/gestures/Reachy_gestures/Key joint values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoln\Documents\Projects\NonAnthroHands_User_Study\data\gestures\Reachy_gestures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8A5922-385A-4D47-B320-0F581873CE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C00DA8-083A-41DE-90D1-746F0589AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{285818F9-1BD3-4F0D-8E91-612AE6A72065}"/>
+    <workbookView xWindow="13872" yWindow="1800" windowWidth="9168" windowHeight="11220" xr2:uid="{285818F9-1BD3-4F0D-8E91-612AE6A72065}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
-  <si>
-    <t>Jaco Gestures:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
   <si>
     <t>Touch up (cartesian):</t>
   </si>
@@ -125,15 +122,9 @@
     <t>Mid position (box)</t>
   </si>
   <si>
-    <t>Mid position (Jaco)</t>
-  </si>
-  <si>
     <t>End position (box)</t>
   </si>
   <si>
-    <t>End position (Jaco)</t>
-  </si>
-  <si>
     <t>Forward/left</t>
   </si>
   <si>
@@ -254,9 +245,6 @@
     <t>(-22,-62,61,-95,62,-43)</t>
   </si>
   <si>
-    <t>(0.16,-.2,.69)</t>
-  </si>
-  <si>
     <t>(17,-30,52,-112,64,45)</t>
   </si>
   <si>
@@ -285,6 +273,24 @@
   </si>
   <si>
     <t>wave always goes last</t>
+  </si>
+  <si>
+    <t>(0.16,-.19,.67)</t>
+  </si>
+  <si>
+    <t>(-33,-55,76,-91,43,-45)</t>
+  </si>
+  <si>
+    <t>Mid position (Reachy)</t>
+  </si>
+  <si>
+    <t>End position (Reachy)</t>
+  </si>
+  <si>
+    <t>(-48,-45,81,-69,36,-45)</t>
+  </si>
+  <si>
+    <t>Reachy Gestures:</t>
   </si>
 </sst>
 </file>
@@ -326,15 +332,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -652,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9CBC5D-5D25-46F3-AB0B-6EBCA30BEFD7}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,59 +674,59 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
       <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
       <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -758,15 +762,15 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="R4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>-17</v>
@@ -798,19 +802,19 @@
       <c r="L5">
         <v>-56</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="R5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -842,19 +846,19 @@
       <c r="L6">
         <v>-78</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>3</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>-34</v>
@@ -886,25 +890,25 @@
       <c r="L7">
         <v>-125</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>4</v>
       </c>
       <c r="P7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="R7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>-23</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>52</v>
@@ -930,25 +934,25 @@
       <c r="L8">
         <v>3</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>5</v>
       </c>
       <c r="P8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>56</v>
+      <c r="C9" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D9">
         <v>-2</v>
@@ -974,275 +978,278 @@
       <c r="L9">
         <v>-8</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <v>6</v>
       </c>
       <c r="P9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="R9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <v>7</v>
       </c>
       <c r="P10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="O11" s="4">
+        <v>4</v>
+      </c>
+      <c r="O11" s="3">
         <v>8</v>
       </c>
       <c r="P11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="4">
+      <c r="O12" s="3">
         <v>9</v>
       </c>
       <c r="P12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="R12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="4">
+        <v>31</v>
+      </c>
+      <c r="O13" s="3">
         <v>10</v>
       </c>
       <c r="P13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="O14" s="4">
+        <v>17</v>
+      </c>
+      <c r="O14" s="3">
         <v>11</v>
       </c>
       <c r="P14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="4">
+        <v>18</v>
+      </c>
+      <c r="O15" s="3">
         <v>12</v>
       </c>
       <c r="P15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="O16" s="4">
+        <v>19</v>
+      </c>
+      <c r="O16" s="3">
         <v>13</v>
       </c>
       <c r="P16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="R16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O17" s="4">
+        <v>20</v>
+      </c>
+      <c r="O17" s="3">
         <v>14</v>
       </c>
       <c r="P17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="R17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18" s="4">
+        <v>21</v>
+      </c>
+      <c r="O18" s="3">
         <v>15</v>
       </c>
       <c r="P18" t="s">
+        <v>74</v>
+      </c>
+      <c r="R18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O19" s="3">
+        <v>16</v>
+      </c>
+      <c r="P19" t="s">
+        <v>33</v>
+      </c>
+      <c r="R19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O20" s="3">
+        <v>17</v>
+      </c>
+      <c r="P20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" t="s">
+        <v>35</v>
+      </c>
+      <c r="S20" t="s">
         <v>78</v>
-      </c>
-      <c r="R18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="O19" s="4">
-        <v>16</v>
-      </c>
-      <c r="P19" t="s">
-        <v>36</v>
-      </c>
-      <c r="R19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="O20" s="4">
-        <v>17</v>
-      </c>
-      <c r="P20" t="s">
-        <v>37</v>
-      </c>
-      <c r="R20" t="s">
-        <v>38</v>
-      </c>
-      <c r="S20" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="O21" s="4">
+        <v>24</v>
+      </c>
+      <c r="O21" s="3">
         <v>18</v>
       </c>
       <c r="P21" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="D22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
         <v>28</v>
       </c>
-      <c r="F22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" t="s">
-        <v>30</v>
-      </c>
       <c r="I22" t="s">
-        <v>31</v>
-      </c>
-      <c r="O22" s="4">
+        <v>82</v>
+      </c>
+      <c r="O22" s="3">
         <v>19</v>
       </c>
       <c r="P22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
         <v>61</v>
       </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>62</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
         <v>63</v>
       </c>
-      <c r="F23" t="s">
+      <c r="I23" t="s">
         <v>64</v>
       </c>
-      <c r="G23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" t="s">
-        <v>67</v>
-      </c>
-      <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
+      <c r="G24" t="s">
         <v>69</v>
       </c>
-      <c r="D24" t="s">
+      <c r="H24" t="s">
         <v>70</v>
       </c>
-      <c r="E24" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>71</v>
       </c>
-      <c r="G24" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" t="s">
-        <v>75</v>
-      </c>
-      <c r="O24" s="5"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="O25" s="5"/>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>